<commit_message>
EPBDS-8247 Implement ability to store description of Conditions and Return and Input data separately from Rules table. Fix bugs.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8247_Conditions_Actions_Returns/EPBDS-8247_Conditions_Actions_Returns_1.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8247_Conditions_Actions_Returns/EPBDS-8247_Conditions_Actions_Returns_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-8247_Conditions_Actions_Returns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B72884-0886-4F7B-A748-3C136E33BA65}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C611DF0-DA41-45DD-AE9E-674899E9EE7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="2235" windowWidth="31875" windowHeight="17670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conditions" sheetId="6" r:id="rId1"/>
@@ -147,9 +147,6 @@
     <t>Return1</t>
   </si>
   <si>
-    <t>SmartRules DoubleValue test6(Double param1)</t>
-  </si>
-  <si>
     <t>Test test6 test6Test</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Test test7 test7Test</t>
   </si>
   <si>
-    <t>SmartRules Collect DoubleValue[] test7(Double param1)</t>
-  </si>
-  <si>
     <t>4,4,4,4,4,4</t>
   </si>
   <si>
@@ -280,6 +274,12 @@
   </si>
   <si>
     <t>Test test9 test9Test</t>
+  </si>
+  <si>
+    <t>SmartRules DoubleValue test6(Integer param1)</t>
+  </si>
+  <si>
+    <t>SmartRules Collect DoubleValue[] test7(Integer param1)</t>
   </si>
 </sst>
 </file>
@@ -498,83 +498,101 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -584,24 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -977,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F354967-CCBB-4C8D-AC6A-190478DBA6AE}">
   <dimension ref="C3:P136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
@@ -996,17 +996,17 @@
   <sheetData>
     <row r="3" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C4" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54"/>
+      <c r="C4" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
       <c r="M4" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
@@ -1032,41 +1032,41 @@
         <v>4</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="3:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46" t="s">
+      <c r="E6" s="43"/>
+      <c r="F6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="35" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="M6" s="34" t="s">
+      <c r="I6" s="53"/>
+      <c r="M6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="O6" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="P6" s="36" t="s">
+      <c r="O6" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="53" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1074,203 +1074,203 @@
       <c r="C7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="36"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="36"/>
+      <c r="D7" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="53"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C8" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46" t="s">
+      <c r="E8" s="43"/>
+      <c r="F8" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="46"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="36"/>
-      <c r="M8" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" s="35" t="s">
+      <c r="G8" s="43"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
+      <c r="M8" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="P8" s="36" t="s">
-        <v>68</v>
+      <c r="O8" s="52"/>
+      <c r="P8" s="53" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C9" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="36"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="36"/>
+        <v>46</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="53"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="53"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46" t="s">
+      <c r="E10" s="43"/>
+      <c r="F10" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="51"/>
-      <c r="M10" s="34" t="s">
+      <c r="I10" s="55"/>
+      <c r="M10" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="N10" s="35" t="s">
+      <c r="N10" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="O10" s="35"/>
-      <c r="P10" s="36"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="53"/>
     </row>
     <row r="11" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="46"/>
-      <c r="H11" s="35" t="s">
+      <c r="E11" s="43"/>
+      <c r="F11" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="43"/>
+      <c r="H11" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="49"/>
+      <c r="I11" s="53"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="57"/>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C12" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="36"/>
+        <v>51</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="53"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C13" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="36"/>
+        <v>52</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="53"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C14" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="36"/>
+        <v>53</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="53"/>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C15" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="46"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="36"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="43"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="53"/>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C16" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="36"/>
+        <v>51</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="53"/>
     </row>
     <row r="17" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="36"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
+        <v>53</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="53"/>
       <c r="M18" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
@@ -1278,20 +1278,20 @@
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C19" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="46"/>
-      <c r="H19" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="36"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="43"/>
+      <c r="H19" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="53"/>
       <c r="M19" s="19" t="s">
         <v>7</v>
       </c>
@@ -1307,70 +1307,70 @@
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C20" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="M20" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="N20" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="O20" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="P20" s="36" t="s">
-        <v>70</v>
+        <v>51</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="M20" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="P20" s="53" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="46"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="36"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="36"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="43"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="53"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="53"/>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="36"/>
-      <c r="M22" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="53"/>
+      <c r="M22" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="N22" s="35" t="s">
+      <c r="N22" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="O22" s="35" t="s">
+      <c r="O22" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="P22" s="36" t="s">
+      <c r="P22" s="53" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1378,49 +1378,49 @@
       <c r="C23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39" t="s">
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="55"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="36"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="54"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="53"/>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M24" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="P24" s="36"/>
+      <c r="M24" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="P24" s="53"/>
     </row>
     <row r="25" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M25" s="50"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="48"/>
-      <c r="P25" s="49"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="57"/>
     </row>
     <row r="28" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C29" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="41"/>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="44"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
@@ -1428,17 +1428,17 @@
         <v>9</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="13"/>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C31" s="45">
-        <v>1</v>
-      </c>
-      <c r="D31" s="46"/>
+      <c r="C31" s="42">
+        <v>1</v>
+      </c>
+      <c r="D31" s="43"/>
       <c r="E31">
         <v>6</v>
       </c>
@@ -1448,119 +1448,119 @@
       <c r="M31" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="N31" s="56" t="s">
+      <c r="N31" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="O31" s="56"/>
+      <c r="O31" s="34"/>
       <c r="P31" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C32" s="45">
+      <c r="C32" s="42">
         <v>2</v>
       </c>
-      <c r="D32" s="46"/>
+      <c r="D32" s="43"/>
       <c r="E32">
         <v>5</v>
       </c>
       <c r="F32" s="4">
         <v>2</v>
       </c>
-      <c r="M32" s="34" t="s">
+      <c r="M32" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="N32" s="56" t="s">
+      <c r="N32" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="O32" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="P32" s="57" t="s">
+      <c r="O32" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="P32" s="36" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C33" s="45">
+      <c r="C33" s="42">
         <v>3</v>
       </c>
-      <c r="D33" s="46"/>
+      <c r="D33" s="43"/>
       <c r="E33">
         <v>4</v>
       </c>
       <c r="F33" s="4">
         <v>3</v>
       </c>
-      <c r="M33" s="34"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="57"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
+      <c r="P33" s="36"/>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C34" s="45">
+      <c r="C34" s="42">
         <v>4</v>
       </c>
-      <c r="D34" s="46"/>
+      <c r="D34" s="43"/>
       <c r="E34">
         <v>3</v>
       </c>
       <c r="F34" s="4">
         <v>4</v>
       </c>
-      <c r="M34" s="34" t="s">
+      <c r="M34" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="N34" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="O34" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P34" s="57" t="s">
-        <v>66</v>
+      <c r="N34" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="O34" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P34" s="36" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C35" s="45">
+      <c r="C35" s="42">
         <v>5</v>
       </c>
-      <c r="D35" s="46"/>
+      <c r="D35" s="43"/>
       <c r="E35">
         <v>2</v>
       </c>
       <c r="F35" s="4">
         <v>5</v>
       </c>
-      <c r="M35" s="34"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="57"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="34"/>
+      <c r="P35" s="36"/>
     </row>
     <row r="36" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="38">
-        <v>6</v>
-      </c>
-      <c r="D36" s="39"/>
+      <c r="C36" s="44">
+        <v>6</v>
+      </c>
+      <c r="D36" s="45"/>
       <c r="E36" s="5">
         <v>1</v>
       </c>
       <c r="F36" s="6">
         <v>6</v>
       </c>
-      <c r="M36" s="34" t="s">
+      <c r="M36" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="N36" s="56" t="s">
+      <c r="N36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="O36" s="56"/>
-      <c r="P36" s="57"/>
+      <c r="O36" s="34"/>
+      <c r="P36" s="36"/>
     </row>
     <row r="37" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M37" s="47"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="59"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="39"/>
     </row>
     <row r="38" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="3:16" x14ac:dyDescent="0.2">
@@ -1572,10 +1572,10 @@
       <c r="F39" s="40"/>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="48" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -1586,10 +1586,10 @@
       </c>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C41" s="45">
-        <v>1</v>
-      </c>
-      <c r="D41" s="46">
+      <c r="C41" s="42">
+        <v>1</v>
+      </c>
+      <c r="D41" s="43">
         <v>1</v>
       </c>
       <c r="E41">
@@ -1600,10 +1600,10 @@
       </c>
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C42" s="45">
+      <c r="C42" s="42">
         <v>2</v>
       </c>
-      <c r="D42" s="46">
+      <c r="D42" s="43">
         <v>2</v>
       </c>
       <c r="E42">
@@ -1614,10 +1614,10 @@
       </c>
     </row>
     <row r="43" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C43" s="45">
+      <c r="C43" s="42">
         <v>3</v>
       </c>
-      <c r="D43" s="46">
+      <c r="D43" s="43">
         <v>3</v>
       </c>
       <c r="E43">
@@ -1628,10 +1628,10 @@
       </c>
     </row>
     <row r="44" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C44" s="45">
+      <c r="C44" s="42">
         <v>4</v>
       </c>
-      <c r="D44" s="46">
+      <c r="D44" s="43">
         <v>4</v>
       </c>
       <c r="E44">
@@ -1642,10 +1642,10 @@
       </c>
     </row>
     <row r="45" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C45" s="45">
+      <c r="C45" s="42">
         <v>5</v>
       </c>
-      <c r="D45" s="46">
+      <c r="D45" s="43">
         <v>5</v>
       </c>
       <c r="E45">
@@ -1656,10 +1656,10 @@
       </c>
     </row>
     <row r="46" spans="3:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="38">
-        <v>6</v>
-      </c>
-      <c r="D46" s="39">
+      <c r="C46" s="44">
+        <v>6</v>
+      </c>
+      <c r="D46" s="45">
         <v>6</v>
       </c>
       <c r="E46" s="5">
@@ -1674,7 +1674,7 @@
       <c r="C49" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="42"/>
+      <c r="D49" s="46"/>
       <c r="E49" s="41"/>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.2">
@@ -1715,7 +1715,7 @@
       <c r="C55" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D55" s="42"/>
+      <c r="D55" s="46"/>
       <c r="E55" s="41"/>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.2">
@@ -1761,51 +1761,51 @@
       <c r="F62" s="40"/>
     </row>
     <row r="63" spans="3:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C63" s="43" t="s">
+      <c r="C63" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="D63" s="44"/>
-      <c r="E63" s="44"/>
+      <c r="D63" s="48"/>
+      <c r="E63" s="48"/>
       <c r="F63" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C64" s="45">
-        <v>1</v>
-      </c>
-      <c r="D64" s="46"/>
-      <c r="E64" s="46"/>
+      <c r="C64" s="42">
+        <v>1</v>
+      </c>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
       <c r="F64" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C65" s="45">
+      <c r="C65" s="42">
         <v>2</v>
       </c>
-      <c r="D65" s="46"/>
-      <c r="E65" s="46"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
       <c r="F65" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C66" s="45">
+      <c r="C66" s="42">
         <v>3</v>
       </c>
-      <c r="D66" s="46"/>
-      <c r="E66" s="46"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="43"/>
       <c r="F66" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="67" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="38">
+      <c r="C67" s="44">
         <v>4</v>
       </c>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
       <c r="F67" s="6">
         <v>4</v>
       </c>
@@ -1844,37 +1844,37 @@
     <row r="79" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C80" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="D80" s="42"/>
-      <c r="E80" s="42"/>
-      <c r="F80" s="42"/>
-      <c r="G80" s="42"/>
+        <v>55</v>
+      </c>
+      <c r="D80" s="46"/>
+      <c r="E80" s="46"/>
+      <c r="F80" s="46"/>
+      <c r="G80" s="46"/>
       <c r="H80" s="41"/>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C81" s="43" t="s">
+      <c r="C81" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D81" s="48"/>
+      <c r="E81" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D81" s="44"/>
-      <c r="E81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="H81" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C82" s="45">
-        <v>1</v>
-      </c>
-      <c r="D82" s="46"/>
+      <c r="C82" s="42">
+        <v>1</v>
+      </c>
+      <c r="D82" s="43"/>
       <c r="E82">
         <v>6</v>
       </c>
@@ -1889,10 +1889,10 @@
       </c>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C83" s="45">
+      <c r="C83" s="42">
         <v>2</v>
       </c>
-      <c r="D83" s="46"/>
+      <c r="D83" s="43"/>
       <c r="E83">
         <v>5</v>
       </c>
@@ -1907,10 +1907,10 @@
       </c>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C84" s="45">
+      <c r="C84" s="42">
         <v>3</v>
       </c>
-      <c r="D84" s="46"/>
+      <c r="D84" s="43"/>
       <c r="E84">
         <v>4</v>
       </c>
@@ -1925,10 +1925,10 @@
       </c>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C85" s="45">
+      <c r="C85" s="42">
         <v>4</v>
       </c>
-      <c r="D85" s="46"/>
+      <c r="D85" s="43"/>
       <c r="E85">
         <v>3</v>
       </c>
@@ -1943,10 +1943,10 @@
       </c>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C86" s="45">
+      <c r="C86" s="42">
         <v>5</v>
       </c>
-      <c r="D86" s="46"/>
+      <c r="D86" s="43"/>
       <c r="E86">
         <v>2</v>
       </c>
@@ -1961,10 +1961,10 @@
       </c>
     </row>
     <row r="87" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="38">
-        <v>6</v>
-      </c>
-      <c r="D87" s="39"/>
+      <c r="C87" s="44">
+        <v>6</v>
+      </c>
+      <c r="D87" s="45"/>
       <c r="E87" s="5">
         <v>1</v>
       </c>
@@ -1981,7 +1981,7 @@
     <row r="91" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="92" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C92" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D92" s="41"/>
     </row>
@@ -2012,37 +2012,37 @@
     <row r="99" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="100" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C100" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D100" s="42"/>
-      <c r="E100" s="42"/>
-      <c r="F100" s="42"/>
-      <c r="G100" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="D100" s="46"/>
+      <c r="E100" s="46"/>
+      <c r="F100" s="46"/>
+      <c r="G100" s="46"/>
       <c r="H100" s="41"/>
     </row>
     <row r="101" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C101" s="43" t="s">
+      <c r="C101" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D101" s="48"/>
+      <c r="E101" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D101" s="44"/>
-      <c r="E101" s="2" t="s">
+      <c r="G101" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F101" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="H101" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="102" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C102" s="45">
-        <v>1</v>
-      </c>
-      <c r="D102" s="46"/>
+      <c r="C102" s="42">
+        <v>1</v>
+      </c>
+      <c r="D102" s="43"/>
       <c r="E102">
         <v>6</v>
       </c>
@@ -2057,10 +2057,10 @@
       </c>
     </row>
     <row r="103" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C103" s="45">
+      <c r="C103" s="42">
         <v>2</v>
       </c>
-      <c r="D103" s="46"/>
+      <c r="D103" s="43"/>
       <c r="E103">
         <v>5</v>
       </c>
@@ -2075,10 +2075,10 @@
       </c>
     </row>
     <row r="104" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C104" s="45">
+      <c r="C104" s="42">
         <v>3</v>
       </c>
-      <c r="D104" s="46"/>
+      <c r="D104" s="43"/>
       <c r="E104">
         <v>4</v>
       </c>
@@ -2093,10 +2093,10 @@
       </c>
     </row>
     <row r="105" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C105" s="45">
+      <c r="C105" s="42">
         <v>4</v>
       </c>
-      <c r="D105" s="46"/>
+      <c r="D105" s="43"/>
       <c r="E105">
         <v>3</v>
       </c>
@@ -2111,10 +2111,10 @@
       </c>
     </row>
     <row r="106" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C106" s="45">
+      <c r="C106" s="42">
         <v>5</v>
       </c>
-      <c r="D106" s="46"/>
+      <c r="D106" s="43"/>
       <c r="E106">
         <v>2</v>
       </c>
@@ -2129,10 +2129,10 @@
       </c>
     </row>
     <row r="107" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C107" s="38">
-        <v>6</v>
-      </c>
-      <c r="D107" s="39"/>
+      <c r="C107" s="44">
+        <v>6</v>
+      </c>
+      <c r="D107" s="45"/>
       <c r="E107" s="5">
         <v>1</v>
       </c>
@@ -2149,7 +2149,7 @@
     <row r="111" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="112" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C112" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D112" s="41"/>
     </row>
@@ -2180,37 +2180,37 @@
     <row r="120" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="121" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C121" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D121" s="42"/>
-      <c r="E121" s="42"/>
-      <c r="F121" s="42"/>
-      <c r="G121" s="42"/>
+        <v>61</v>
+      </c>
+      <c r="D121" s="46"/>
+      <c r="E121" s="46"/>
+      <c r="F121" s="46"/>
+      <c r="G121" s="46"/>
       <c r="H121" s="41"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C122" s="43" t="s">
+      <c r="C122" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D122" s="48"/>
+      <c r="E122" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D122" s="44"/>
-      <c r="E122" s="2" t="s">
+      <c r="G122" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F122" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G122" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="H122" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C123" s="45">
-        <v>1</v>
-      </c>
-      <c r="D123" s="46"/>
+      <c r="C123" s="42">
+        <v>1</v>
+      </c>
+      <c r="D123" s="43"/>
       <c r="E123">
         <v>6</v>
       </c>
@@ -2225,10 +2225,10 @@
       </c>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C124" s="45">
+      <c r="C124" s="42">
         <v>2</v>
       </c>
-      <c r="D124" s="46"/>
+      <c r="D124" s="43"/>
       <c r="E124">
         <v>5</v>
       </c>
@@ -2243,10 +2243,10 @@
       </c>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C125" s="45">
+      <c r="C125" s="42">
         <v>3</v>
       </c>
-      <c r="D125" s="46"/>
+      <c r="D125" s="43"/>
       <c r="E125">
         <v>4</v>
       </c>
@@ -2261,10 +2261,10 @@
       </c>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C126" s="45">
+      <c r="C126" s="42">
         <v>4</v>
       </c>
-      <c r="D126" s="46"/>
+      <c r="D126" s="43"/>
       <c r="E126">
         <v>3</v>
       </c>
@@ -2279,10 +2279,10 @@
       </c>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C127" s="45">
+      <c r="C127" s="42">
         <v>5</v>
       </c>
-      <c r="D127" s="46"/>
+      <c r="D127" s="43"/>
       <c r="E127">
         <v>2</v>
       </c>
@@ -2297,10 +2297,10 @@
       </c>
     </row>
     <row r="128" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C128" s="38">
-        <v>6</v>
-      </c>
-      <c r="D128" s="39"/>
+      <c r="C128" s="44">
+        <v>6</v>
+      </c>
+      <c r="D128" s="45"/>
       <c r="E128" s="5">
         <v>1</v>
       </c>
@@ -2317,7 +2317,7 @@
     <row r="132" spans="3:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="133" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C133" s="40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D133" s="41"/>
     </row>
@@ -2347,15 +2347,88 @@
     </row>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N34:N35"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="N32:N33"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="P32:P33"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:O9"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="C121:H121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="N10:P11"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="M24:N25"/>
+    <mergeCell ref="O24:P25"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C80:H80"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H19:I22"/>
+    <mergeCell ref="F11:G14"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H11:I18"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H6:I9"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="M36:M37"/>
     <mergeCell ref="N36:P37"/>
     <mergeCell ref="C112:D112"/>
@@ -2380,88 +2453,15 @@
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C85:D85"/>
     <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H6:I9"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H19:I22"/>
-    <mergeCell ref="F11:G14"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H11:I18"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="C121:H121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="N10:P11"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="M24:N25"/>
-    <mergeCell ref="O24:P25"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C80:H80"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:O9"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="P34:P35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2472,8 +2472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63C529D-8F6D-4385-8ECE-0B2A69A63EA5}">
   <dimension ref="B3:R86"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18:L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2498,7 +2498,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="13"/>
       <c r="L4" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
@@ -2508,25 +2508,25 @@
       <c r="R4" s="22"/>
     </row>
     <row r="5" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="65" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="65"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="66"/>
-      <c r="L5" s="63" t="s">
+      <c r="H5" s="63"/>
+      <c r="L5" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="64"/>
+      <c r="M5" s="65"/>
       <c r="N5" s="27" t="s">
         <v>5</v>
       </c>
@@ -2540,152 +2540,152 @@
       <c r="R5" s="24"/>
     </row>
     <row r="6" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="67"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
       <c r="F6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="66"/>
-      <c r="L6" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="M6" s="35"/>
+      <c r="H6" s="63"/>
+      <c r="L6" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="52"/>
       <c r="N6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35" t="s">
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="R6" s="36"/>
+      <c r="R6" s="53"/>
     </row>
     <row r="7" spans="2:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="67"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="65" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="65"/>
+      <c r="E7" s="62"/>
       <c r="F7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="66"/>
-      <c r="L7" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="M7" s="35"/>
+      <c r="G7" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="63"/>
+      <c r="L7" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="52"/>
       <c r="N7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="36"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="53"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
       <c r="F8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="66"/>
-      <c r="L8" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="35"/>
+      <c r="G8" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="63"/>
+      <c r="L8" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="52"/>
       <c r="N8" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="36"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="53"/>
     </row>
     <row r="9" spans="2:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="39"/>
+      <c r="B9" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="45"/>
       <c r="F9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="L9" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" s="35"/>
+      <c r="H9" s="54"/>
+      <c r="L9" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="52"/>
       <c r="N9" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="36"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="53"/>
     </row>
     <row r="10" spans="2:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L10" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="M10" s="48"/>
+      <c r="L10" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="56"/>
       <c r="N10" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48" t="s">
+      <c r="O10" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="49"/>
+      <c r="R10" s="57"/>
     </row>
     <row r="15" spans="2:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="41"/>
-      <c r="L16" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="62"/>
+      <c r="L16" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="68"/>
     </row>
     <row r="17" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="44"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
@@ -2695,22 +2695,22 @@
       <c r="L17" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="46" t="s">
+      <c r="M17" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="N17" s="43"/>
+      <c r="O17" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N17" s="46"/>
-      <c r="O17" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q17" s="4" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="46"/>
+      <c r="C18" s="43"/>
       <c r="D18">
         <v>6</v>
       </c>
@@ -2720,23 +2720,23 @@
       <c r="L18" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M18" s="46" t="s">
+      <c r="M18" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="51" t="s">
+      <c r="N18" s="43"/>
+      <c r="O18" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="55" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="46"/>
+      <c r="C19" s="43"/>
       <c r="D19">
         <v>5</v>
       </c>
@@ -2744,17 +2744,17 @@
         <v>2</v>
       </c>
       <c r="L19" s="32"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="51"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="55"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="46"/>
+      <c r="C20" s="43"/>
       <c r="D20">
         <v>4</v>
       </c>
@@ -2764,21 +2764,21 @@
       <c r="L20" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="46" t="s">
+      <c r="M20" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="46"/>
-      <c r="Q20" s="51" t="s">
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="55" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="46"/>
+      <c r="C21" s="43"/>
       <c r="D21">
         <v>3</v>
       </c>
@@ -2786,17 +2786,17 @@
         <v>4</v>
       </c>
       <c r="L21" s="32"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="46"/>
-      <c r="Q21" s="51"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="55"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="46"/>
+      <c r="C22" s="43"/>
       <c r="D22">
         <v>2</v>
       </c>
@@ -2806,21 +2806,21 @@
       <c r="L22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M22" s="46" t="s">
+      <c r="M22" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="51" t="s">
-        <v>80</v>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="55" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="39"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="5">
         <v>1</v>
       </c>
@@ -2828,26 +2828,26 @@
         <v>6</v>
       </c>
       <c r="L23" s="32"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="51"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="55"/>
     </row>
     <row r="24" spans="2:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L24" s="33"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="55"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="54"/>
     </row>
     <row r="27" spans="2:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="42"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="41"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.2">
@@ -2889,15 +2889,15 @@
       <c r="B36" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
       <c r="E36" s="41"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="44"/>
+      <c r="C37" s="48"/>
       <c r="D37" s="2" t="s">
         <v>10</v>
       </c>
@@ -2906,10 +2906,10 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="46"/>
+      <c r="C38" s="43"/>
       <c r="D38">
         <v>6</v>
       </c>
@@ -2918,10 +2918,10 @@
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="46"/>
+      <c r="C39" s="43"/>
       <c r="D39">
         <v>5</v>
       </c>
@@ -2930,10 +2930,10 @@
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="46"/>
+      <c r="C40" s="43"/>
       <c r="D40">
         <v>4</v>
       </c>
@@ -2942,10 +2942,10 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="46"/>
+      <c r="C41" s="43"/>
       <c r="D41">
         <v>3</v>
       </c>
@@ -2954,10 +2954,10 @@
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="45" t="s">
+      <c r="B42" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="46"/>
+      <c r="C42" s="43"/>
       <c r="D42">
         <v>2</v>
       </c>
@@ -2966,10 +2966,10 @@
       </c>
     </row>
     <row r="43" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="39"/>
+      <c r="C43" s="45"/>
       <c r="D43" s="5">
         <v>1</v>
       </c>
@@ -2982,7 +2982,7 @@
       <c r="B47" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="42"/>
+      <c r="C47" s="46"/>
       <c r="D47" s="41"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
@@ -3021,7 +3021,7 @@
     <row r="53" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="40" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C54" s="41"/>
     </row>
@@ -3084,7 +3084,7 @@
     <row r="64" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B65" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C65" s="41"/>
     </row>
@@ -3115,7 +3115,7 @@
     <row r="71" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B72" s="40" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C72" s="41"/>
     </row>
@@ -3178,7 +3178,7 @@
     <row r="82" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B83" s="40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C83" s="41"/>
     </row>
@@ -3203,11 +3203,47 @@
         <v>2</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="M22:P24"/>
+    <mergeCell ref="Q22:Q24"/>
+    <mergeCell ref="L16:Q16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N19"/>
+    <mergeCell ref="O18:P19"/>
+    <mergeCell ref="M20:P21"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O6:P7"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="Q6:R9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B54:C54"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B36:E36"/>
@@ -3224,42 +3260,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O6:P7"/>
-    <mergeCell ref="O8:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="Q6:R9"/>
-    <mergeCell ref="M22:P24"/>
-    <mergeCell ref="Q22:Q24"/>
-    <mergeCell ref="L16:Q16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N19"/>
-    <mergeCell ref="O18:P19"/>
-    <mergeCell ref="M20:P21"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="Q20:Q21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3282,24 +3282,24 @@
     <row r="4" spans="3:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D5" s="70"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>